<commit_message>
upload inital boiler plate for database and client table creation
</commit_message>
<xml_diff>
--- a/Group1 Mini Project 2 database design.xlsx
+++ b/Group1 Mini Project 2 database design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Documents\KODEGO\WD35\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Documents\KODEGO\WD35\week 6to10\mini-project-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51F29A7-520A-4DA2-8D40-7A0796D185C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2015B9-780C-4E22-BBB3-CAC4583FBF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1635" windowWidth="20385" windowHeight="13860" xr2:uid="{FD11F99D-59BA-4732-BBB4-F2EBC31D6E9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{FD11F99D-59BA-4732-BBB4-F2EBC31D6E9C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>clientFName</t>
   </si>
@@ -50,54 +50,18 @@
     <t>package</t>
   </si>
   <si>
-    <t>foodBuffet</t>
-  </si>
-  <si>
-    <t>foodPlated</t>
-  </si>
-  <si>
-    <t>flowerArrangement</t>
-  </si>
-  <si>
-    <t>tablesChairs</t>
-  </si>
-  <si>
-    <t>invitations</t>
-  </si>
-  <si>
-    <t>lightSounds</t>
-  </si>
-  <si>
     <t>Client Info</t>
   </si>
   <si>
     <t>package Inclusions</t>
   </si>
   <si>
-    <t>decor</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
     <t>eventType</t>
   </si>
   <si>
-    <t>birthday</t>
-  </si>
-  <si>
-    <t>anniversary</t>
-  </si>
-  <si>
-    <t>wedding</t>
-  </si>
-  <si>
-    <t>christening</t>
-  </si>
-  <si>
-    <t>christmasParty</t>
-  </si>
-  <si>
     <t>startTime</t>
   </si>
   <si>
@@ -107,9 +71,6 @@
     <t>location</t>
   </si>
   <si>
-    <t>eventContractor</t>
-  </si>
-  <si>
     <t>Leocadios's Events Database design</t>
   </si>
   <si>
@@ -149,9 +110,6 @@
     <t>inclusionId</t>
   </si>
   <si>
-    <t>food</t>
-  </si>
-  <si>
     <t>Inclusions</t>
   </si>
   <si>
@@ -167,13 +125,136 @@
     <t>tunnel design</t>
   </si>
   <si>
-    <t>stage</t>
-  </si>
-  <si>
-    <t>backdrop</t>
-  </si>
-  <si>
-    <t>ceiling design</t>
+    <t>Event: Wedding, Birthday, Others.</t>
+  </si>
+  <si>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event Place: </t>
+  </si>
+  <si>
+    <t>Church Set-up: Standard, Premium, No</t>
+  </si>
+  <si>
+    <t>Guest: 100pax, 100-150pax, 150-200pax, 200pax-300 pax</t>
+  </si>
+  <si>
+    <t>Videographer: Yes, No</t>
+  </si>
+  <si>
+    <t>Photographer: Yes, No</t>
+  </si>
+  <si>
+    <t>Host: Yes, No</t>
+  </si>
+  <si>
+    <t>Event Organizer: Yes, No</t>
+  </si>
+  <si>
+    <t>Backdrop: Yes, No</t>
+  </si>
+  <si>
+    <t>Stage: Yes, No</t>
+  </si>
+  <si>
+    <t>Ceiling Decoration: Standard, Premium, No</t>
+  </si>
+  <si>
+    <t>Tunnel Design: Yes, No</t>
+  </si>
+  <si>
+    <t>LED Wall: Yes, No</t>
+  </si>
+  <si>
+    <t>Lights and Sounds: Yes, No</t>
+  </si>
+  <si>
+    <t>Food: Yes, No</t>
+  </si>
+  <si>
+    <t>Pica-Pica: Station: 100pax, 100-150pax, 150-200pax, 200pax-300 pax</t>
+  </si>
+  <si>
+    <t>Wedding</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>others</t>
+  </si>
+  <si>
+    <t>inclusions</t>
+  </si>
+  <si>
+    <t>Church setup standard</t>
+  </si>
+  <si>
+    <t>Church setup premium</t>
+  </si>
+  <si>
+    <t>Church setup none</t>
+  </si>
+  <si>
+    <t>guest 100</t>
+  </si>
+  <si>
+    <t>guest 151-200</t>
+  </si>
+  <si>
+    <t>guest 201-300</t>
+  </si>
+  <si>
+    <t>videographer</t>
+  </si>
+  <si>
+    <t>photographer</t>
+  </si>
+  <si>
+    <t>event organizer</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>Backdrop</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Ceiling décor standard</t>
+  </si>
+  <si>
+    <t>ceiling décor premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ceiling décor none</t>
+  </si>
+  <si>
+    <t>LED wall</t>
+  </si>
+  <si>
+    <t>Lights&amp;Sounds</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>guest 101-150</t>
+  </si>
+  <si>
+    <t>Pica-pica station 100</t>
+  </si>
+  <si>
+    <t>Pica-pica station 151-200</t>
+  </si>
+  <si>
+    <t>Pica-pica station 101-150</t>
+  </si>
+  <si>
+    <t>Pica-pica station 201-250</t>
   </si>
 </sst>
 </file>
@@ -252,14 +333,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,7 +646,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -574,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6423BFF-4EAA-4AF7-BF3B-525F46F6B6D3}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,330 +666,397 @@
     <col min="7" max="12" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="N7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="N9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="N11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="2"/>
+      <c r="N12" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="N16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="N17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="N18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="N19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20">
         <v>3</v>
       </c>
-      <c r="C20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21">
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
-    </row>
-    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="N32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="S32" s="4"/>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="N33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:19" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="N34" t="s">
+        <v>1</v>
+      </c>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="N35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+      <c r="N36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="N37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>61</v>
+      </c>
+      <c r="N38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="N39" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>0</v>
-      </c>
-      <c r="D35" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" t="s">
-        <v>8</v>
-      </c>
-      <c r="F39" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D47" t="s">
-        <v>45</v>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>